<commit_message>
reporte pdf y generacion
</commit_message>
<xml_diff>
--- a/tp1/report/reglas_validacion.xlsx
+++ b/tp1/report/reglas_validacion.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -816,6 +816,23 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>r27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>paciente mayor de edad</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>!is.na(fechaid) &amp; !is.na(interview) &amp; (interval(fechaid, interview) / years(1)) &gt;= 18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>